<commit_message>
cap nhat luong thang 9
</commit_message>
<xml_diff>
--- a/Data/092018/nhanvien.xlsx
+++ b/Data/092018/nhanvien.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C098CBBB-191F-44C4-8BC9-59438F967749}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04A6FE3B-0F01-4AE0-9A90-DA17EF67D215}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>Hai</t>
   </si>
@@ -52,9 +52,6 @@
     <t>Tuan</t>
   </si>
   <si>
-    <t>Thuy</t>
-  </si>
-  <si>
     <t>Dung</t>
   </si>
   <si>
@@ -62,6 +59,12 @@
   </si>
   <si>
     <t>Duong</t>
+  </si>
+  <si>
+    <t>*|Thuy:0.7</t>
+  </si>
+  <si>
+    <t>*|Duong:0.7</t>
   </si>
 </sst>
 </file>
@@ -391,19 +394,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A11" sqref="A11"/>
+      <selection pane="bottomRight" activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="9" width="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -505,7 +509,7 @@
         <v>0.5</v>
       </c>
       <c r="K3" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -534,7 +538,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7">
         <v>4500</v>
@@ -572,7 +576,7 @@
         <v>0.7</v>
       </c>
       <c r="K8" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -642,41 +646,6 @@
         <v>0.7</v>
       </c>
       <c r="K10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11">
-        <v>3000</v>
-      </c>
-      <c r="C11">
-        <v>0.01</v>
-      </c>
-      <c r="D11">
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="E11">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="F11">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="G11">
-        <v>1.7000000000000001E-2</v>
-      </c>
-      <c r="H11">
-        <v>1.9E-2</v>
-      </c>
-      <c r="I11">
-        <v>0.02</v>
-      </c>
-      <c r="J11">
-        <v>0.7</v>
-      </c>
-      <c r="K11" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>